<commit_message>
Working scraper + some bugs removed + default values in sheet through api
</commit_message>
<xml_diff>
--- a/etm_ref/etm_inputs_clean.xlsx
+++ b/etm_ref/etm_inputs_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\0 Thesis\05 GIT\etm-api\etm_ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{138B3EA2-CF8B-4AF4-919C-C08CEC229A91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44025572-038A-4493-A2F0-D1A7E175FBD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{029C1739-8AAC-4CC1-A472-02F73E3EBBF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{029C1739-8AAC-4CC1-A472-02F73E3EBBF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5284,8 +5284,8 @@
   <dimension ref="A1:F484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B489" sqref="B489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6199,7 +6199,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>160</v>
       </c>
@@ -6212,7 +6212,7 @@
       <c r="D54" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="3" t="s">
         <v>1286</v>
       </c>
     </row>
@@ -11552,7 +11552,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="371" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>992</v>
       </c>
@@ -11565,7 +11565,7 @@
       <c r="D371" t="s">
         <v>1289</v>
       </c>
-      <c r="E371" s="1" t="s">
+      <c r="E371" s="2" t="s">
         <v>1288</v>
       </c>
     </row>
@@ -11654,7 +11654,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="377" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>992</v>
       </c>
@@ -11667,7 +11667,7 @@
       <c r="D377" t="s">
         <v>1289</v>
       </c>
-      <c r="E377" s="1" t="s">
+      <c r="E377" s="2" t="s">
         <v>1288</v>
       </c>
     </row>
@@ -11756,7 +11756,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="383" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>992</v>
       </c>
@@ -11769,7 +11769,7 @@
       <c r="D383" t="s">
         <v>1289</v>
       </c>
-      <c r="E383" s="1" t="s">
+      <c r="E383" s="2" t="s">
         <v>1288</v>
       </c>
     </row>
@@ -11858,7 +11858,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="389" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>992</v>
       </c>
@@ -11871,7 +11871,7 @@
       <c r="D389" t="s">
         <v>1289</v>
       </c>
-      <c r="E389" s="1" t="s">
+      <c r="E389" s="2" t="s">
         <v>1288</v>
       </c>
     </row>
@@ -11960,7 +11960,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="395" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>992</v>
       </c>
@@ -11973,7 +11973,7 @@
       <c r="D395" t="s">
         <v>1289</v>
       </c>
-      <c r="E395" s="1" t="s">
+      <c r="E395" s="2" t="s">
         <v>1288</v>
       </c>
     </row>
@@ -12062,7 +12062,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="401" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>992</v>
       </c>
@@ -12075,7 +12075,7 @@
       <c r="D401" t="s">
         <v>1289</v>
       </c>
-      <c r="E401" s="1" t="s">
+      <c r="E401" s="2" t="s">
         <v>1288</v>
       </c>
     </row>
@@ -12188,7 +12188,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="410" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>1070</v>
       </c>
@@ -12201,7 +12201,7 @@
       <c r="D410" t="s">
         <v>1289</v>
       </c>
-      <c r="E410" s="1" t="s">
+      <c r="E410" s="2" t="s">
         <v>1290</v>
       </c>
     </row>
@@ -12375,7 +12375,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="421" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>413</v>
       </c>
@@ -12388,7 +12388,7 @@
       <c r="D421" t="s">
         <v>1289</v>
       </c>
-      <c r="E421" s="1" t="s">
+      <c r="E421" s="2" t="s">
         <v>1293</v>
       </c>
     </row>
@@ -12477,7 +12477,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="427" spans="1:5" ht="405" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>413</v>
       </c>
@@ -12490,7 +12490,7 @@
       <c r="D427" t="s">
         <v>1298</v>
       </c>
-      <c r="E427" s="1" t="s">
+      <c r="E427" s="2" t="s">
         <v>1294</v>
       </c>
     </row>
@@ -12848,7 +12848,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="449" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>263</v>
       </c>
@@ -12861,7 +12861,7 @@
       <c r="D449" t="s">
         <v>1289</v>
       </c>
-      <c r="E449" s="1" t="s">
+      <c r="E449" s="2" t="s">
         <v>1295</v>
       </c>
     </row>

</xml_diff>